<commit_message>
Add 2 sites, del 5
</commit_message>
<xml_diff>
--- a/xlsx/himki.xlsx
+++ b/xlsx/himki.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4200000</v>
+        <v>2455000</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4200000</v>
+        <v>2455000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1490000</v>
+        <v>1390000</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1490000</v>
+        <v>1390000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1690000</v>
+        <v>1440000</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1690000</v>
+        <v>1440000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2195000</v>
+        <v>1790000</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2195000</v>
+        <v>1790000</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1894,7 +1894,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1713000</v>
+        <v>1499000</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1713000</v>
+        <v>1499000</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1993,7 +1993,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1040000</v>
+        <v>1119900</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2001,7 +2001,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>1040000</v>
+        <v>1119900</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2054000</v>
+        <v>1899000</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>2054000</v>
+        <v>1899000</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2599000</v>
+        <v>1990000</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>2599000</v>
+        <v>1990000</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -5293,7 +5293,7 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>1528000</v>
+        <v>2490000</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -5301,7 +5301,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>1528000</v>
+        <v>2490000</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -5345,7 +5345,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>486</t>
+          <t>484</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -5355,30 +5355,30 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>CX-50</t>
+          <t>CX-5 New</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>2490000</v>
+        <v>2690000</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/mazda/cx-50/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-5_new/</t>
         </is>
       </c>
       <c r="F150" t="n">
-        <v>2490000</v>
+        <v>2690000</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/mazda/cx-50/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-5_new/</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>479</t>
+          <t>486</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -5388,63 +5388,63 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-50</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>2973000</v>
+        <v>2490000</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/mazda/cx-9/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-50/</t>
         </is>
       </c>
       <c r="F151" t="n">
-        <v>2973000</v>
+        <v>2490000</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/mazda/cx-9/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-50/</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>509</t>
+          <t>479</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Moskvich</t>
+          <t>Mazda</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>1299000</v>
+        <v>2973000</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/moskvich/3/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-9/</t>
         </is>
       </c>
       <c r="F152" t="n">
-        <v>1299000</v>
+        <v>2973000</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/moskvich/3/</t>
+          <t>https://autogansa.ru/cars/mazda/cx-9/</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>509</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -5454,63 +5454,63 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1899000</v>
+        <v>1299000</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/moskvich/6/</t>
+          <t>https://autogansa.ru/cars/moskvich/3/</t>
         </is>
       </c>
       <c r="F153" t="n">
-        <v>1899000</v>
+        <v>1299000</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/moskvich/6/</t>
+          <t>https://autogansa.ru/cars/moskvich/3/</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>511</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Moskvich</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Murano</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>2590000</v>
+        <v>1899000</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/murano/</t>
+          <t>https://autogansa.ru/cars/moskvich/6/</t>
         </is>
       </c>
       <c r="F154" t="n">
-        <v>2590000</v>
+        <v>1899000</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/murano/</t>
+          <t>https://autogansa.ru/cars/moskvich/6/</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>517</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -5520,30 +5520,30 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Qashqai</t>
+          <t>Murano</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>790000</v>
+        <v>2590000</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/qashqai_new/</t>
+          <t>https://autogansa.ru/cars/nissan/murano/</t>
         </is>
       </c>
       <c r="F155" t="n">
-        <v>790000</v>
+        <v>2590000</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/qashqai_new/</t>
+          <t>https://autogansa.ru/cars/nissan/murano/</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>520</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -5553,30 +5553,30 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Terrano</t>
+          <t>Qashqai</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>890000</v>
+        <v>790000</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/terrano/</t>
+          <t>https://autogansa.ru/cars/nissan/qashqai_new/</t>
         </is>
       </c>
       <c r="F156" t="n">
-        <v>890000</v>
+        <v>790000</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/terrano/</t>
+          <t>https://autogansa.ru/cars/nissan/qashqai_new/</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>522</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -5586,63 +5586,63 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>X-trail New</t>
+          <t>Terrano</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>855000</v>
+        <v>890000</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/x_trail/</t>
+          <t>https://autogansa.ru/cars/nissan/terrano/</t>
         </is>
       </c>
       <c r="F157" t="n">
-        <v>855000</v>
+        <v>890000</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/nissan/x_trail/</t>
+          <t>https://autogansa.ru/cars/nissan/terrano/</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>OMODA</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>C5</t>
+          <t>X-trail New</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>1199000</v>
+        <v>855000</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/c5/</t>
+          <t>https://autogansa.ru/cars/nissan/x_trail/</t>
         </is>
       </c>
       <c r="F158" t="n">
-        <v>1199000</v>
+        <v>855000</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/c5/</t>
+          <t>https://autogansa.ru/cars/nissan/x_trail/</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>820</t>
+          <t>525</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -5652,30 +5652,30 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>C5 New</t>
+          <t>C5</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>1399000</v>
+        <v>1199000</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/c5_new/</t>
+          <t>https://autogansa.ru/cars/omoda/c5/</t>
         </is>
       </c>
       <c r="F159" t="n">
-        <v>1399000</v>
+        <v>1199000</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/c5_new/</t>
+          <t>https://autogansa.ru/cars/omoda/c5/</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>526</t>
+          <t>820</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -5685,30 +5685,30 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>S5</t>
+          <t>C5 New</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1099000</v>
+        <v>1399000</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/s5/</t>
+          <t>https://autogansa.ru/cars/omoda/c5_new/</t>
         </is>
       </c>
       <c r="F160" t="n">
-        <v>1099000</v>
+        <v>1399000</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/s5/</t>
+          <t>https://autogansa.ru/cars/omoda/c5_new/</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>527</t>
+          <t>526</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -5718,96 +5718,96 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>S5 GT</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1869900</v>
+        <v>1099000</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/s5_gt/</t>
+          <t>https://autogansa.ru/cars/omoda/s5/</t>
         </is>
       </c>
       <c r="F161" t="n">
-        <v>1869900</v>
+        <v>1099000</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/omoda/s5_gt/</t>
+          <t>https://autogansa.ru/cars/omoda/s5/</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>527</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Oting</t>
+          <t>OMODA</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Paladin</t>
+          <t>S5 GT</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>3199000</v>
+        <v>1869900</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/oting/paladin/</t>
+          <t>https://autogansa.ru/cars/omoda/s5_gt/</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>3199000</v>
+        <v>1869900</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/oting/paladin/</t>
+          <t>https://autogansa.ru/cars/omoda/s5_gt/</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>541</t>
+          <t>537</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Peugeot</t>
+          <t>Oting</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>2008 New</t>
+          <t>Paladin</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>2649000</v>
+        <v>3199000</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/2008/</t>
+          <t>https://autogansa.ru/cars/oting/paladin/</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>2649000</v>
+        <v>3199000</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/2008/</t>
+          <t>https://autogansa.ru/cars/oting/paladin/</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>786</t>
+          <t>541</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -5817,30 +5817,30 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>4008</t>
+          <t>2008 New</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>3299000</v>
+        <v>2649000</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/4008/</t>
+          <t>https://autogansa.ru/cars/peugeot/2008/</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>3299000</v>
+        <v>2649000</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/4008/</t>
+          <t>https://autogansa.ru/cars/peugeot/2008/</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>543</t>
+          <t>786</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5850,63 +5850,63 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>5008 New</t>
+          <t>4008</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>3499000</v>
+        <v>3299000</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/5008/</t>
+          <t>https://autogansa.ru/cars/peugeot/4008/</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>3499000</v>
+        <v>3299000</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/peugeot/5008/</t>
+          <t>https://autogansa.ru/cars/peugeot/4008/</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>548</t>
+          <t>543</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Ravon</t>
+          <t>Peugeot</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Gentra</t>
+          <t>5008 New</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>917000</v>
+        <v>3499000</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/gentra/</t>
+          <t>https://autogansa.ru/cars/peugeot/5008/</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>917000</v>
+        <v>3499000</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/gentra/</t>
+          <t>https://autogansa.ru/cars/peugeot/5008/</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>545</t>
+          <t>548</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5916,30 +5916,30 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Nexia R3</t>
+          <t>Gentra</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>805000</v>
+        <v>917000</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/nexia_r3/</t>
+          <t>https://autogansa.ru/cars/ravon/gentra/</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>805000</v>
+        <v>917000</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/nexia_r3/</t>
+          <t>https://autogansa.ru/cars/ravon/gentra/</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>546</t>
+          <t>545</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5949,30 +5949,30 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>Nexia R3</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>1049000</v>
+        <v>805000</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/r2/</t>
+          <t>https://autogansa.ru/cars/ravon/nexia_r3/</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>1049000</v>
+        <v>805000</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/r2/</t>
+          <t>https://autogansa.ru/cars/ravon/nexia_r3/</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>547</t>
+          <t>546</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -5982,63 +5982,63 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>831000</v>
+        <v>1049000</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/r4/</t>
+          <t>https://autogansa.ru/cars/ravon/r2/</t>
         </is>
       </c>
       <c r="F169" t="n">
-        <v>831000</v>
+        <v>1049000</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/ravon/r4/</t>
+          <t>https://autogansa.ru/cars/ravon/r2/</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>547</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Renault</t>
+          <t>Ravon</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Arkana</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>890000</v>
+        <v>831000</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/arkana/</t>
+          <t>https://autogansa.ru/cars/ravon/r4/</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>890000</v>
+        <v>831000</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/arkana/</t>
+          <t>https://autogansa.ru/cars/ravon/r4/</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -6048,30 +6048,30 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Duster New</t>
+          <t>Arkana</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>650000</v>
+        <v>890000</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/duster_new/</t>
+          <t>https://autogansa.ru/cars/renault/arkana/</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>650000</v>
+        <v>890000</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/duster_new/</t>
+          <t>https://autogansa.ru/cars/renault/arkana/</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>556</t>
+          <t>555</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -6081,30 +6081,30 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Kaptur</t>
+          <t>Duster New</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>890000</v>
+        <v>650000</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/kaptur/</t>
+          <t>https://autogansa.ru/cars/renault/duster_new/</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>890000</v>
+        <v>650000</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/kaptur/</t>
+          <t>https://autogansa.ru/cars/renault/duster_new/</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>558</t>
+          <t>556</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -6114,30 +6114,30 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Kaptur</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>690000</v>
+        <v>890000</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/logan/</t>
+          <t>https://autogansa.ru/cars/renault/kaptur/</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>690000</v>
+        <v>890000</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/logan/</t>
+          <t>https://autogansa.ru/cars/renault/kaptur/</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>559</t>
+          <t>558</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -6147,30 +6147,30 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Logan Stepway</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>740000</v>
+        <v>690000</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/logan_stepway/</t>
+          <t>https://autogansa.ru/cars/renault/logan/</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>740000</v>
+        <v>690000</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/logan_stepway/</t>
+          <t>https://autogansa.ru/cars/renault/logan/</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>559</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -6180,30 +6180,30 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Sandero</t>
+          <t>Logan Stepway</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>730000</v>
+        <v>740000</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/sandero/</t>
+          <t>https://autogansa.ru/cars/renault/logan_stepway/</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>730000</v>
+        <v>740000</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/sandero/</t>
+          <t>https://autogansa.ru/cars/renault/logan_stepway/</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>566</t>
+          <t>565</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -6213,96 +6213,96 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Sandero Stepway</t>
+          <t>Sandero</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>790000</v>
+        <v>730000</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/sandero_stepway/</t>
+          <t>https://autogansa.ru/cars/renault/sandero/</t>
         </is>
       </c>
       <c r="F176" t="n">
-        <v>790000</v>
+        <v>730000</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/renault/sandero_stepway/</t>
+          <t>https://autogansa.ru/cars/renault/sandero/</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>566</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Rox</t>
+          <t>Renault</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>Sandero Stepway</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>7949000</v>
+        <v>790000</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/rox/01/</t>
+          <t>https://autogansa.ru/cars/renault/sandero_stepway/</t>
         </is>
       </c>
       <c r="F177" t="n">
-        <v>7949000</v>
+        <v>790000</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/rox/01/</t>
+          <t>https://autogansa.ru/cars/renault/sandero_stepway/</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>611</t>
+          <t>789</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>SWM</t>
+          <t>Rox</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>G01</t>
+          <t>01</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>990000</v>
+        <v>6529000</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g01/</t>
+          <t>https://autogansa.ru/cars/rox/01/</t>
         </is>
       </c>
       <c r="F178" t="n">
-        <v>990000</v>
+        <v>6529000</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g01/</t>
+          <t>https://autogansa.ru/cars/rox/01/</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>612</t>
+          <t>611</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -6312,30 +6312,30 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>G01F</t>
+          <t>G01</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>1119000</v>
+        <v>990000</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g01f/</t>
+          <t>https://autogansa.ru/cars/swm/g01/</t>
         </is>
       </c>
       <c r="F179" t="n">
-        <v>1119000</v>
+        <v>990000</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g01f/</t>
+          <t>https://autogansa.ru/cars/swm/g01/</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>613</t>
+          <t>612</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -6345,63 +6345,63 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>G05 Pro</t>
+          <t>G01F</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>1249000</v>
+        <v>1119000</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g05_pro/</t>
+          <t>https://autogansa.ru/cars/swm/g01f/</t>
         </is>
       </c>
       <c r="F180" t="n">
-        <v>1249000</v>
+        <v>1119000</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/swm/g05_pro/</t>
+          <t>https://autogansa.ru/cars/swm/g01f/</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>571</t>
+          <t>613</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Skoda</t>
+          <t>SWM</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Karoq</t>
+          <t>G05 Pro</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>1499000</v>
+        <v>1249000</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/karoq/</t>
+          <t>https://autogansa.ru/cars/swm/g05_pro/</t>
         </is>
       </c>
       <c r="F181" t="n">
-        <v>1499000</v>
+        <v>1249000</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/karoq/</t>
+          <t>https://autogansa.ru/cars/swm/g05_pro/</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>574</t>
+          <t>571</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -6411,30 +6411,30 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Kodiaq</t>
+          <t>Karoq</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>1899000</v>
+        <v>1499000</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/kodiaq/</t>
+          <t>https://autogansa.ru/cars/skoda/karoq/</t>
         </is>
       </c>
       <c r="F182" t="n">
-        <v>1899000</v>
+        <v>1499000</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/kodiaq/</t>
+          <t>https://autogansa.ru/cars/skoda/karoq/</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>578</t>
+          <t>574</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Octavia</t>
+          <t>Kodiaq</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -6452,7 +6452,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/octavia/</t>
+          <t>https://autogansa.ru/cars/skoda/kodiaq/</t>
         </is>
       </c>
       <c r="F183" t="n">
@@ -6460,14 +6460,14 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/octavia/</t>
+          <t>https://autogansa.ru/cars/skoda/kodiaq/</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>581</t>
+          <t>578</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -6477,30 +6477,30 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Rapid</t>
+          <t>Octavia</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>979000</v>
+        <v>1899000</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/rapid/</t>
+          <t>https://autogansa.ru/cars/skoda/octavia/</t>
         </is>
       </c>
       <c r="F184" t="n">
-        <v>979000</v>
+        <v>1899000</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/rapid/</t>
+          <t>https://autogansa.ru/cars/skoda/octavia/</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>585</t>
+          <t>581</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -6510,63 +6510,63 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Superb</t>
+          <t>Rapid</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>2199000</v>
+        <v>979000</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/superb/</t>
+          <t>https://autogansa.ru/cars/skoda/rapid/</t>
         </is>
       </c>
       <c r="F185" t="n">
-        <v>2199000</v>
+        <v>979000</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/skoda/superb/</t>
+          <t>https://autogansa.ru/cars/skoda/rapid/</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>585</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Solaris</t>
+          <t>Skoda</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>Superb</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>1950000</v>
+        <v>2199000</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/hc/</t>
+          <t>https://autogansa.ru/cars/skoda/superb/</t>
         </is>
       </c>
       <c r="F186" t="n">
-        <v>1950000</v>
+        <v>2199000</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/hc/</t>
+          <t>https://autogansa.ru/cars/skoda/superb/</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>595</t>
+          <t>594</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -6576,30 +6576,30 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>HS</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>1218000</v>
+        <v>1950000</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/hs/</t>
+          <t>https://autogansa.ru/cars/solaris/hc/</t>
         </is>
       </c>
       <c r="F187" t="n">
-        <v>1218000</v>
+        <v>1950000</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/hs/</t>
+          <t>https://autogansa.ru/cars/solaris/hc/</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>596</t>
+          <t>595</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -6609,30 +6609,30 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>KRS</t>
+          <t>HS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>1380000</v>
+        <v>1218000</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/krs/</t>
+          <t>https://autogansa.ru/cars/solaris/hs/</t>
         </is>
       </c>
       <c r="F188" t="n">
-        <v>1380000</v>
+        <v>1218000</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/krs/</t>
+          <t>https://autogansa.ru/cars/solaris/hs/</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>597</t>
+          <t>596</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -6642,63 +6642,63 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>KRX</t>
+          <t>KRS</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>1481000</v>
+        <v>1380000</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/krx/</t>
+          <t>https://autogansa.ru/cars/solaris/krs/</t>
         </is>
       </c>
       <c r="F189" t="n">
-        <v>1481000</v>
+        <v>1380000</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/solaris/krx/</t>
+          <t>https://autogansa.ru/cars/solaris/krs/</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>821</t>
+          <t>597</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Soueast</t>
+          <t>Solaris</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>S07</t>
+          <t>KRX</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>2049000</v>
+        <v>1481000</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/soueast/s07/</t>
+          <t>https://autogansa.ru/cars/solaris/krx/</t>
         </is>
       </c>
       <c r="F190" t="n">
-        <v>2049000</v>
+        <v>1481000</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/soueast/s07/</t>
+          <t>https://autogansa.ru/cars/solaris/krx/</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>822</t>
+          <t>821</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -6708,63 +6708,63 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>S09</t>
+          <t>S07</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>2399000</v>
+        <v>2049000</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/soueast/s09/</t>
+          <t>https://autogansa.ru/cars/soueast/s07/</t>
         </is>
       </c>
       <c r="F191" t="n">
-        <v>2399000</v>
+        <v>2049000</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/soueast/s09/</t>
+          <t>https://autogansa.ru/cars/soueast/s07/</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>822</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>TANK</t>
+          <t>Soueast</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>S09</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>2499000</v>
+        <v>2399000</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/tank/300/</t>
+          <t>https://autogansa.ru/cars/soueast/s09/</t>
         </is>
       </c>
       <c r="F192" t="n">
-        <v>2499000</v>
+        <v>2399000</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/tank/300/</t>
+          <t>https://autogansa.ru/cars/soueast/s09/</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>615</t>
+          <t>614</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -6774,63 +6774,63 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>4899000</v>
+        <v>2499000</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/tank/500/</t>
+          <t>https://autogansa.ru/cars/tank/300/</t>
         </is>
       </c>
       <c r="F193" t="n">
-        <v>4899000</v>
+        <v>2499000</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/tank/500/</t>
+          <t>https://autogansa.ru/cars/tank/300/</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>623</t>
+          <t>615</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>TANK</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>CH-R</t>
+          <t>500</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>1865000</v>
+        <v>4899000</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/c-hr/</t>
+          <t>https://autogansa.ru/cars/tank/500/</t>
         </is>
       </c>
       <c r="F194" t="n">
-        <v>1865000</v>
+        <v>4899000</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/c-hr/</t>
+          <t>https://autogansa.ru/cars/tank/500/</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>621</t>
+          <t>623</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -6840,30 +6840,30 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>CH-R</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>2940000</v>
+        <v>1865000</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/camry/</t>
+          <t>https://autogansa.ru/cars/toyota/c-hr/</t>
         </is>
       </c>
       <c r="F195" t="n">
-        <v>2940000</v>
+        <v>1865000</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/camry/</t>
+          <t>https://autogansa.ru/cars/toyota/c-hr/</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>617</t>
+          <t>621</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -6873,30 +6873,30 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>1767000</v>
+        <v>2940000</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/corolla/</t>
+          <t>https://autogansa.ru/cars/toyota/camry/</t>
         </is>
       </c>
       <c r="F196" t="n">
-        <v>1767000</v>
+        <v>2940000</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/corolla/</t>
+          <t>https://autogansa.ru/cars/toyota/camry/</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>625</t>
+          <t>617</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -6906,30 +6906,30 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Highlander</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>6190000</v>
+        <v>1767000</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/highlander/</t>
+          <t>https://autogansa.ru/cars/toyota/corolla/</t>
         </is>
       </c>
       <c r="F197" t="n">
-        <v>6190000</v>
+        <v>1767000</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/highlander/</t>
+          <t>https://autogansa.ru/cars/toyota/corolla/</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>629</t>
+          <t>625</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -6939,30 +6939,30 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Land Cruiser 300</t>
+          <t>Highlander</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>8724000</v>
+        <v>6190000</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_300/</t>
+          <t>https://autogansa.ru/cars/toyota/highlander/</t>
         </is>
       </c>
       <c r="F198" t="n">
-        <v>8724000</v>
+        <v>6190000</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_300/</t>
+          <t>https://autogansa.ru/cars/toyota/highlander/</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>740</t>
+          <t>629</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -6972,30 +6972,30 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Land Cruiser 300 GR-Sport</t>
+          <t>Land Cruiser 300</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>11456500</v>
+        <v>8724000</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_300_gr_sport/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_300/</t>
         </is>
       </c>
       <c r="F199" t="n">
-        <v>11456500</v>
+        <v>8724000</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_300_gr_sport/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_300/</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>741</t>
+          <t>740</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -7005,30 +7005,30 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Land Cruiser Prado New</t>
+          <t>Land Cruiser 300 GR-Sport</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>7690000</v>
+        <v>11456500</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_250_prado/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_300_gr_sport/</t>
         </is>
       </c>
       <c r="F200" t="n">
-        <v>7690000</v>
+        <v>11456500</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/land_cruiser_250_prado/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_300_gr_sport/</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>741</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -7038,63 +7038,63 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>RAV4</t>
+          <t>Land Cruiser Prado New</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>2729000</v>
+        <v>7690000</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/rav4/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_250_prado/</t>
         </is>
       </c>
       <c r="F201" t="n">
-        <v>2729000</v>
+        <v>7690000</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/toyota/rav4/</t>
+          <t>https://autogansa.ru/cars/toyota/land_cruiser_250_prado/</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>620</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>UAZ</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>RAV4</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>1499000</v>
+        <v>2729000</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/uaz/patriot/</t>
+          <t>https://autogansa.ru/cars/toyota/rav4/</t>
         </is>
       </c>
       <c r="F202" t="n">
-        <v>1499000</v>
+        <v>2729000</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/uaz/patriot/</t>
+          <t>https://autogansa.ru/cars/toyota/rav4/</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>637</t>
+          <t>634</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -7104,7 +7104,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -7112,7 +7112,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/uaz/pikap/</t>
+          <t>https://autogansa.ru/cars/uaz/patriot/</t>
         </is>
       </c>
       <c r="F203" t="n">
@@ -7120,47 +7120,47 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/uaz/pikap/</t>
+          <t>https://autogansa.ru/cars/uaz/patriot/</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>645</t>
+          <t>637</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>UAZ</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Jetta</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>1285000</v>
+        <v>1499000</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/jetta/</t>
+          <t>https://autogansa.ru/cars/uaz/pikap/</t>
         </is>
       </c>
       <c r="F204" t="n">
-        <v>1285000</v>
+        <v>1499000</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/jetta/</t>
+          <t>https://autogansa.ru/cars/uaz/pikap/</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>645</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -7170,30 +7170,30 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>Jetta</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>2438000</v>
+        <v>1285000</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/passat/</t>
+          <t>https://autogansa.ru/cars/volkswagen/jetta/</t>
         </is>
       </c>
       <c r="F205" t="n">
-        <v>2438000</v>
+        <v>1285000</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/passat/</t>
+          <t>https://autogansa.ru/cars/volkswagen/jetta/</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>652</t>
+          <t>649</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -7203,30 +7203,30 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>899000</v>
+        <v>2438000</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/polo/</t>
+          <t>https://autogansa.ru/cars/volkswagen/passat/</t>
         </is>
       </c>
       <c r="F206" t="n">
-        <v>899000</v>
+        <v>2438000</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/polo/</t>
+          <t>https://autogansa.ru/cars/volkswagen/passat/</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>655</t>
+          <t>652</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -7236,54 +7236,87 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Teramont</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>6990000</v>
+        <v>899000</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/teramont/</t>
+          <t>https://autogansa.ru/cars/volkswagen/polo/</t>
         </is>
       </c>
       <c r="F207" t="n">
-        <v>6990000</v>
+        <v>899000</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>https://autogansa.ru/cars/volkswagen/teramont/</t>
+          <t>https://autogansa.ru/cars/volkswagen/polo/</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
+          <t>655</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Teramont</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>6990000</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>https://autogansa.ru/cars/volkswagen/teramont/</t>
+        </is>
+      </c>
+      <c r="F208" t="n">
+        <v>6990000</v>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>https://autogansa.ru/cars/volkswagen/teramont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
           <t>657</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
+      <c r="B209" t="inlineStr">
         <is>
           <t>Volkswagen</t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
+      <c r="C209" t="inlineStr">
         <is>
           <t>Tiguan</t>
         </is>
       </c>
-      <c r="D208" t="n">
+      <c r="D209" t="n">
         <v>1990000</v>
       </c>
-      <c r="E208" t="inlineStr">
+      <c r="E209" t="inlineStr">
         <is>
           <t>https://autogansa.ru/cars/volkswagen/tiguan/</t>
         </is>
       </c>
-      <c r="F208" t="n">
+      <c r="F209" t="n">
         <v>1990000</v>
       </c>
-      <c r="G208" t="inlineStr">
+      <c r="G209" t="inlineStr">
         <is>
           <t>https://autogansa.ru/cars/volkswagen/tiguan/</t>
         </is>

</xml_diff>